<commit_message>
release notes and rretrospection
</commit_message>
<xml_diff>
--- a/Deskify Documents/Product-Backlog.xlsx
+++ b/Deskify Documents/Product-Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shwetha.b\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1F6CD2-2CA7-47E6-B38D-40AB7446A6DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B4A733-784B-4792-8283-6955EBC65553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1662,7 +1662,7 @@
   <dimension ref="A1:K138"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F57" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F63" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="H129" sqref="H129"/>

</xml_diff>